<commit_message>
added redme files and reorganised
</commit_message>
<xml_diff>
--- a/3_genomeWide_relationships/PCAs/eigenvalues.xlsx
+++ b/3_genomeWide_relationships/PCAs/eigenvalues.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sstankow/Documents/GitHub/Littorina_reproductive_mode/genomeWide_relationships/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sstankow/Documents/GitHub/Littorina_reproductive_mode/3_genomeWide_relationships/PCAs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A93B001-CCF8-4642-B0A6-E7FBF9E78820}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62252217-4C87-F54E-BE26-57E4B7D9021B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37960" yWindow="-1340" windowWidth="27240" windowHeight="15800" xr2:uid="{A0C03716-DBF2-4C40-95F2-F18D376FA5C4}"/>
   </bookViews>
@@ -27,28 +27,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>full</t>
-  </si>
-  <si>
     <t>full_perc</t>
-  </si>
-  <si>
-    <t>pruned</t>
   </si>
   <si>
     <t>pruned_perc</t>
   </si>
   <si>
-    <t>full_downsampled</t>
-  </si>
-  <si>
     <t>full_downsampled_perc</t>
   </si>
   <si>
-    <t>pruned_downsampled</t>
+    <t>pruned_downsampled_perc</t>
   </si>
   <si>
-    <t>pruned_downsampled_perc</t>
+    <t>full_eig</t>
+  </si>
+  <si>
+    <t>pruned_eig</t>
+  </si>
+  <si>
+    <t>full_downsampled_eig</t>
+  </si>
+  <si>
+    <t>pruned_downsampled_eig</t>
   </si>
 </sst>
 </file>
@@ -410,39 +410,40 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>